<commit_message>
can parse and edit existing todo.txt files
</commit_message>
<xml_diff>
--- a/to_do.xlsx
+++ b/to_do.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>task</t>
   </si>
@@ -40,37 +40,43 @@
     <t>poc</t>
   </si>
   <si>
-    <t>a</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>2021-12-22</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>2021-12-21</t>
-  </si>
-  <si>
-    <t>@aa</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>2021-12-29</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>2021-12-22</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>+test</t>
-  </si>
-  <si>
-    <t>e</t>
+    <t>this is task one (32 characters)</t>
+  </si>
+  <si>
+    <t>2021-01-10</t>
+  </si>
+  <si>
+    <t>this task has a long description so that we can see how tasks with a really long description looks when the user interface is resized (expanded or condensed) to fit on the screen, really long descriptions must mean the task is complicated (255 characters)</t>
+  </si>
+  <si>
+    <t>test task, predate</t>
+  </si>
+  <si>
+    <t>2020-01-08</t>
+  </si>
+  <si>
+    <t>projectA</t>
+  </si>
+  <si>
+    <t>this is a new task</t>
+  </si>
+  <si>
+    <t>this is task two, it has a little bit more text (64 characters)</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -494,74 +500,95 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
export additions and keyboard shortcuts
</commit_message>
<xml_diff>
--- a/to_do.xlsx
+++ b/to_do.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>task</t>
   </si>
@@ -40,43 +40,37 @@
     <t>poc</t>
   </si>
   <si>
+    <t>test one should be checked</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>2021-12-28</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>test two should not be checked</t>
+  </si>
+  <si>
     <t>test</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>2021-12-22</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>this is task one (32 characters)</t>
-  </si>
-  <si>
-    <t>2021-01-10</t>
-  </si>
-  <si>
-    <t>this task has a long description so that we can see how tasks with a really long description looks when the user interface is resized (expanded or condensed) to fit on the screen, really long descriptions must mean the task is complicated (255 characters)</t>
-  </si>
-  <si>
-    <t>test task, predate</t>
-  </si>
-  <si>
-    <t>2020-01-08</t>
-  </si>
-  <si>
-    <t>projectA</t>
-  </si>
-  <si>
-    <t>this is a new task</t>
-  </si>
-  <si>
-    <t>this is task two, it has a little bit more text (64 characters)</t>
+    <t>full</t>
+  </si>
+  <si>
+    <t>2022-02-02</t>
+  </si>
+  <si>
+    <t>new_sprint</t>
+  </si>
+  <si>
+    <t>new_poc</t>
   </si>
 </sst>
 </file>
@@ -453,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -489,7 +483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -499,96 +493,94 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>